<commit_message>
fixed Afrique occ franc in countries
</commit_message>
<xml_diff>
--- a/Liste mots cles.xlsx
+++ b/Liste mots cles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pays" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="252">
   <si>
     <t>PAYS</t>
   </si>
@@ -745,6 +745,9 @@
   </si>
   <si>
     <t>Afrique</t>
+  </si>
+  <si>
+    <t>Afrique Occidentale française</t>
   </si>
   <si>
     <t>France Grande-Bretagne</t>
@@ -921,14 +924,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.0851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.5185185185185"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8703703703704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.3777777777778"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.0851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.8666666666667"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.1074074074074"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5555555555556"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.162962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.6740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2692,19 +2695,19 @@
   </sheetPr>
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.0851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.4148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.8703703703704"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="30.3777777777778"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.0851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.8666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.5555555555556"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="31.162962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.6740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2842,7 +2845,7 @@
         <v>31</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>32</v>
+        <v>241</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>24</v>
@@ -2866,7 +2869,7 @@
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>240</v>
@@ -2886,7 +2889,7 @@
         <v>38</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>32</v>
+        <v>241</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>24</v>
@@ -2954,7 +2957,7 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>240</v>
@@ -2974,7 +2977,7 @@
         <v>55</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>32</v>
+        <v>241</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>24</v>
@@ -2997,7 +3000,7 @@
         <v>58</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>32</v>
+        <v>241</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>24</v>
@@ -3020,7 +3023,7 @@
         <v>60</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>32</v>
+        <v>241</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>24</v>
@@ -3133,7 +3136,7 @@
         <v>73</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>32</v>
+        <v>241</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>24</v>
@@ -3177,7 +3180,7 @@
         <v>78</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>32</v>
+        <v>241</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>24</v>
@@ -3311,7 +3314,7 @@
         <v>93</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>13</v>
@@ -3334,7 +3337,7 @@
         <v>96</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>13</v>
@@ -3698,7 +3701,7 @@
         <v>171</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E45" s="6" t="n">
         <v>26018</v>
@@ -3719,7 +3722,7 @@
         <v>24</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E46" s="6" t="n">
         <v>19672</v>
@@ -3738,7 +3741,7 @@
         <v>13</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E47" s="6" t="n">
         <v>17394</v>
@@ -3757,7 +3760,7 @@
         <v>181</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E48" s="6" t="n">
         <v>18259</v>
@@ -3778,7 +3781,7 @@
         <v>24</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E49" s="6" t="n">
         <v>18098</v>
@@ -3797,7 +3800,7 @@
         <v>13</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E50" s="6" t="n">
         <v>21063</v>
@@ -3816,7 +3819,7 @@
         <v>13</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E51" s="6" t="n">
         <v>17536</v>
@@ -3835,7 +3838,7 @@
         <v>13</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E52" s="6" t="n">
         <v>17393</v>
@@ -3854,7 +3857,7 @@
         <v>197</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E53" s="6" t="n">
         <v>16987</v>
@@ -3873,7 +3876,7 @@
         <v>13</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E54" s="6" t="n">
         <v>26441</v>
@@ -3894,7 +3897,7 @@
         <v>24</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E55" s="6" t="n">
         <v>19925</v>
@@ -3928,17 +3931,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3948,22 +3951,22 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the list with Congo
</commit_message>
<xml_diff>
--- a/Liste mots cles.xlsx
+++ b/Liste mots cles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pays" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="258">
   <si>
     <t>PAYS</t>
   </si>
@@ -759,10 +759,25 @@
     <t>Afrique Occidentale française|Dahomey</t>
   </si>
   <si>
+    <t>Afrique [É|E]quatoriale française</t>
+  </si>
+  <si>
     <t>Afrique de l'Est Britannique</t>
   </si>
   <si>
     <t>Asie</t>
+  </si>
+  <si>
+    <t>__Inde</t>
+  </si>
+  <si>
+    <t>Inde </t>
+  </si>
+  <si>
+    <t>Congo-Kinshasa|Congo-Léopoldville</t>
+  </si>
+  <si>
+    <t>Congo-Brazzaville</t>
   </si>
   <si>
     <t>TERMES GENERAUX</t>
@@ -927,14 +942,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.8666666666667"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.1074074074074"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5555555555556"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.162962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.6740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.6518518518518"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.6962962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.2407407407407"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9444444444444"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.3592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2703703703704"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2696,21 +2711,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C37" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F58" activeCellId="0" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.8666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.5555555555556"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="31.162962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.6740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.6518518518518"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.0814814814815"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.2407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="31.9444444444444"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.3592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.2703703703704"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3069,8 +3084,8 @@
       <c r="A17" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>65</v>
+      <c r="B17" s="0" t="s">
+        <v>245</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>24</v>
@@ -3092,8 +3107,8 @@
       <c r="A18" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>65</v>
+      <c r="B18" s="0" t="s">
+        <v>245</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>24</v>
@@ -3115,8 +3130,8 @@
       <c r="A19" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>65</v>
+      <c r="B19" s="0" t="s">
+        <v>245</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>24</v>
@@ -3317,7 +3332,7 @@
         <v>93</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>13</v>
@@ -3340,7 +3355,7 @@
         <v>96</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>13</v>
@@ -3704,7 +3719,7 @@
         <v>171</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E45" s="6" t="n">
         <v>26018</v>
@@ -3725,7 +3740,7 @@
         <v>24</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E46" s="6" t="n">
         <v>19672</v>
@@ -3737,14 +3752,16 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B47" s="3"/>
+        <v>248</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>249</v>
+      </c>
       <c r="C47" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E47" s="6" t="n">
         <v>17394</v>
@@ -3763,7 +3780,7 @@
         <v>181</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E48" s="6" t="n">
         <v>18259</v>
@@ -3784,7 +3801,7 @@
         <v>24</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E49" s="6" t="n">
         <v>18098</v>
@@ -3803,7 +3820,7 @@
         <v>13</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E50" s="6" t="n">
         <v>21063</v>
@@ -3822,7 +3839,7 @@
         <v>13</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E51" s="6" t="n">
         <v>17536</v>
@@ -3841,7 +3858,7 @@
         <v>13</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E52" s="6" t="n">
         <v>17393</v>
@@ -3860,7 +3877,7 @@
         <v>197</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E53" s="6" t="n">
         <v>16987</v>
@@ -3879,7 +3896,7 @@
         <v>13</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E54" s="6" t="n">
         <v>26441</v>
@@ -3900,7 +3917,7 @@
         <v>24</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E55" s="6" t="n">
         <v>19925</v>
@@ -3909,6 +3926,42 @@
         <v>1954</v>
       </c>
       <c r="G55" s="3"/>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="E56" s="6"/>
+      <c r="F56" s="0" t="n">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="E57" s="6"/>
+      <c r="F57" s="0" t="n">
+        <v>1960</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3934,17 +3987,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.2703703703704"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3954,22 +4007,22 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the list to contain RegEx only
</commit_message>
<xml_diff>
--- a/Liste mots cles.xlsx
+++ b/Liste mots cles.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="286">
   <si>
     <t>PAYS</t>
   </si>
@@ -726,7 +726,7 @@
     <t>name</t>
   </si>
   <si>
-    <t>other</t>
+    <t>RegEx</t>
   </si>
   <si>
     <t>colonist</t>
@@ -747,37 +747,121 @@
     <t>Afrique</t>
   </si>
   <si>
-    <t>Afrique Occidentale française</t>
+    <t>Côte-de-l'Or|Ghana</t>
+  </si>
+  <si>
+    <t>Afrique Occidentale française|Guinée</t>
   </si>
   <si>
     <t>France Grande-Bretagne</t>
   </si>
   <si>
+    <t>Afrique Occidentale française|Sénégal</t>
+  </si>
+  <si>
+    <t>Protectorat malgache|Madagascar</t>
+  </si>
+  <si>
     <t>Italie Grande-Bretagne</t>
   </si>
   <si>
-    <t>Afrique Occidentale française|Dahomey</t>
-  </si>
-  <si>
-    <t>Afrique [É|E]quatoriale française</t>
-  </si>
-  <si>
-    <t>Afrique de l'Est Britannique</t>
+    <t>Afrique Occidentale française|Dahomey|Bénin</t>
+  </si>
+  <si>
+    <t>Afrique Occidentale française|Niger</t>
+  </si>
+  <si>
+    <t>Afrique Occidentale française|Burkina Faso</t>
+  </si>
+  <si>
+    <t>Afrique [É|E]quatoriale française|Tchad</t>
+  </si>
+  <si>
+    <t>Afrique [É|E]quatoriale française|République centrafricaine</t>
+  </si>
+  <si>
+    <t>Afrique [É|E]quatoriale française|Gabon</t>
+  </si>
+  <si>
+    <t>Afrique Occidentale française|Mali([\s.,;]|en)</t>
+  </si>
+  <si>
+    <t>Nig[é|e]ria</t>
+  </si>
+  <si>
+    <t>Afrique Occidentale française|Mauritanie</t>
+  </si>
+  <si>
+    <t>Tanganyika|Tanzanie</t>
+  </si>
+  <si>
+    <t>Ruanda-Urundi|Rwanda</t>
+  </si>
+  <si>
+    <t>Ruanda-Urundi|Burundi</t>
+  </si>
+  <si>
+    <t>Afrique de l'Est Britannique|Ouganda</t>
+  </si>
+  <si>
+    <t>Afrique de l'Est Britannique|Kenya</t>
+  </si>
+  <si>
+    <t>Nyasaland|Malawi</t>
+  </si>
+  <si>
+    <t>Rhodésie du nord|Zambie</t>
+  </si>
+  <si>
+    <t>Bechuanaland|Botswana</t>
+  </si>
+  <si>
+    <t>Basutoland|Lesotho</t>
+  </si>
+  <si>
+    <t>Guinée (espagnole|équatoriale)</t>
+  </si>
+  <si>
+    <t>Guinée (portugaise|-Bissau)</t>
+  </si>
+  <si>
+    <t>Afrique orientale portugaise|Mozambique</t>
+  </si>
+  <si>
+    <t>Territoire français des Afars et des Issas|Djibouti</t>
+  </si>
+  <si>
+    <t>Rhodésie du Sud|Zimbabwe</t>
+  </si>
+  <si>
+    <t>Afrique du sud-ouest|Namibie</t>
+  </si>
+  <si>
+    <t>Sahara (espagnol|occidental)</t>
   </si>
   <si>
     <t>Asie</t>
   </si>
   <si>
-    <t>__Inde</t>
+    <t>Indochine|Cambodge</t>
   </si>
   <si>
     <t>Inde </t>
   </si>
   <si>
-    <t>Congo-Kinshasa|Congo-Léopoldville</t>
+    <t>Indochine|Laos</t>
+  </si>
+  <si>
+    <t>Indochine|Viêt Nam</t>
+  </si>
+  <si>
+    <t>Congo(-Kinshasa|-Léopoldville| belge)</t>
   </si>
   <si>
     <t>Congo-Brazzaville</t>
+  </si>
+  <si>
+    <t>Afrique [É|E]quatoriale française|Congo-Brazzaville</t>
   </si>
   <si>
     <t>TERMES GENERAUX</t>
@@ -888,7 +972,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -917,6 +1001,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -942,14 +1030,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.6518518518518"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.6962962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.2407407407407"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9444444444444"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.3592592592593"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.337037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2814814814815"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.8296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.6333333333333"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.0481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2713,19 +2801,19 @@
   </sheetPr>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C37" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F58" activeCellId="0" sqref="F58"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B58" activeCellId="0" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.6518518518518"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.0814814814815"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.2407407407407"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="31.9444444444444"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.3592592592593"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.337037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.4037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.8296296296296"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="32.6333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.0481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2755,7 +2843,9 @@
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
@@ -2776,7 +2866,9 @@
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
@@ -2797,7 +2889,9 @@
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="C4" s="3" t="s">
         <v>24</v>
       </c>
@@ -2818,7 +2912,9 @@
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="C5" s="3" t="s">
         <v>24</v>
       </c>
@@ -2840,7 +2936,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>241</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
@@ -2863,7 +2959,7 @@
         <v>31</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>24</v>
@@ -2885,9 +2981,11 @@
       <c r="A8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="C8" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>240</v>
@@ -2907,7 +3005,7 @@
         <v>38</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>24</v>
@@ -2929,7 +3027,9 @@
       <c r="A10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="C10" s="3" t="s">
         <v>24</v>
       </c>
@@ -2951,7 +3051,7 @@
         <v>43</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>44</v>
+        <v>245</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>24</v>
@@ -2973,9 +3073,11 @@
       <c r="A12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="C12" s="3" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>240</v>
@@ -2995,7 +3097,7 @@
         <v>55</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>24</v>
@@ -3018,7 +3120,7 @@
         <v>58</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>24</v>
@@ -3041,7 +3143,7 @@
         <v>60</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>24</v>
@@ -3063,7 +3165,9 @@
       <c r="A16" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="C16" s="3" t="s">
         <v>24</v>
       </c>
@@ -3085,7 +3189,7 @@
         <v>64</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>24</v>
@@ -3108,7 +3212,7 @@
         <v>67</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>24</v>
@@ -3131,7 +3235,7 @@
         <v>71</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>24</v>
@@ -3154,7 +3258,7 @@
         <v>73</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>24</v>
@@ -3176,7 +3280,9 @@
       <c r="A21" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="3"/>
+      <c r="B21" s="3" t="s">
+        <v>254</v>
+      </c>
       <c r="C21" s="3" t="s">
         <v>13</v>
       </c>
@@ -3198,7 +3304,7 @@
         <v>78</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>24</v>
@@ -3220,7 +3326,9 @@
       <c r="A23" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="C23" s="3" t="s">
         <v>13</v>
       </c>
@@ -3242,7 +3350,7 @@
         <v>82</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>83</v>
+        <v>256</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>13</v>
@@ -3265,7 +3373,7 @@
         <v>85</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>86</v>
+        <v>257</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>48</v>
@@ -3288,7 +3396,7 @@
         <v>89</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>86</v>
+        <v>258</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>48</v>
@@ -3310,7 +3418,9 @@
       <c r="A27" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B27" s="3"/>
+      <c r="B27" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="C27" s="3" t="s">
         <v>24</v>
       </c>
@@ -3332,7 +3442,7 @@
         <v>93</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>13</v>
@@ -3355,7 +3465,7 @@
         <v>96</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>13</v>
@@ -3378,7 +3488,7 @@
         <v>98</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>99</v>
+        <v>261</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>13</v>
@@ -3401,7 +3511,7 @@
         <v>101</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>102</v>
+        <v>262</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>13</v>
@@ -3423,7 +3533,9 @@
       <c r="A32" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B32" s="3"/>
+      <c r="B32" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="C32" s="3" t="s">
         <v>13</v>
       </c>
@@ -3445,7 +3557,7 @@
         <v>106</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>107</v>
+        <v>263</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>13</v>
@@ -3468,7 +3580,7 @@
         <v>109</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>110</v>
+        <v>264</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>13</v>
@@ -3490,7 +3602,9 @@
       <c r="A35" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B35" s="3"/>
+      <c r="B35" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="C35" s="3" t="s">
         <v>13</v>
       </c>
@@ -3511,8 +3625,8 @@
       <c r="A36" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>115</v>
+      <c r="B36" s="7" t="s">
+        <v>265</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>116</v>
@@ -3535,7 +3649,7 @@
         <v>118</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>119</v>
+        <v>266</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>120</v>
@@ -3558,7 +3672,7 @@
         <v>122</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>123</v>
+        <v>267</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>120</v>
@@ -3580,7 +3694,9 @@
       <c r="A39" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B39" s="3"/>
+      <c r="B39" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="C39" s="3" t="s">
         <v>120</v>
       </c>
@@ -3601,7 +3717,9 @@
       <c r="A40" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B40" s="3"/>
+      <c r="B40" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="C40" s="3" t="s">
         <v>120</v>
       </c>
@@ -3623,7 +3741,7 @@
         <v>129</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>130</v>
+        <v>268</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>24</v>
@@ -3646,7 +3764,7 @@
         <v>132</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>133</v>
+        <v>269</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>13</v>
@@ -3669,7 +3787,7 @@
         <v>135</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>136</v>
+        <v>270</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>12</v>
@@ -3691,8 +3809,8 @@
       <c r="A44" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>139</v>
+      <c r="B44" s="7" t="s">
+        <v>271</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>116</v>
@@ -3714,12 +3832,14 @@
       <c r="A45" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B45" s="3"/>
+      <c r="B45" s="3" t="s">
+        <v>170</v>
+      </c>
       <c r="C45" s="3" t="s">
         <v>171</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="E45" s="6" t="n">
         <v>26018</v>
@@ -3734,13 +3854,13 @@
         <v>173</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>174</v>
+        <v>273</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="E46" s="6" t="n">
         <v>19672</v>
@@ -3752,16 +3872,16 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>248</v>
+        <v>178</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>249</v>
+        <v>274</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="E47" s="6" t="n">
         <v>17394</v>
@@ -3775,12 +3895,14 @@
       <c r="A48" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B48" s="3"/>
+      <c r="B48" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="C48" s="3" t="s">
         <v>181</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="E48" s="6" t="n">
         <v>18259</v>
@@ -3795,13 +3917,13 @@
         <v>187</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>174</v>
+        <v>275</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="E49" s="6" t="n">
         <v>18098</v>
@@ -3815,12 +3937,14 @@
       <c r="A50" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B50" s="3"/>
+      <c r="B50" s="3" t="s">
+        <v>189</v>
+      </c>
       <c r="C50" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="E50" s="6" t="n">
         <v>21063</v>
@@ -3834,12 +3958,14 @@
       <c r="A51" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B51" s="3"/>
+      <c r="B51" s="3" t="s">
+        <v>193</v>
+      </c>
       <c r="C51" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="E51" s="6" t="n">
         <v>17536</v>
@@ -3853,12 +3979,14 @@
       <c r="A52" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B52" s="3"/>
+      <c r="B52" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="C52" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="E52" s="6" t="n">
         <v>17393</v>
@@ -3872,12 +4000,14 @@
       <c r="A53" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B53" s="3"/>
+      <c r="B53" s="3" t="s">
+        <v>196</v>
+      </c>
       <c r="C53" s="3" t="s">
         <v>197</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="E53" s="6" t="n">
         <v>16987</v>
@@ -3891,12 +4021,14 @@
       <c r="A54" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="B54" s="3"/>
+      <c r="B54" s="3" t="s">
+        <v>201</v>
+      </c>
       <c r="C54" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="E54" s="6" t="n">
         <v>26441</v>
@@ -3911,13 +4043,13 @@
         <v>203</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>174</v>
+        <v>276</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="E55" s="6" t="n">
         <v>19925</v>
@@ -3932,7 +4064,7 @@
         <v>47</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>250</v>
+        <v>277</v>
       </c>
       <c r="C56" s="0" t="s">
         <v>48</v>
@@ -3947,10 +4079,10 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>245</v>
+        <v>279</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>24</v>
@@ -3987,17 +4119,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>252</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>253</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4007,22 +4139,22 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>254</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>255</v>
+        <v>283</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>256</v>
+        <v>284</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>257</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates for the metrics
</commit_message>
<xml_diff>
--- a/Liste mots cles.xlsx
+++ b/Liste mots cles.xlsx
@@ -846,7 +846,7 @@
     <t>Indochine|Cambodge</t>
   </si>
   <si>
-    <t>Inde </t>
+    <t>Inde[\s.,;']</t>
   </si>
   <si>
     <t>Indochine|Laos</t>
@@ -1030,14 +1030,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.562962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.337037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2814814814815"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.8296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.6333333333333"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.0481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.1222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.8703703703704"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.5148148148148"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.4148148148148"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.6333333333333"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2801,19 +2799,18 @@
   </sheetPr>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B58" activeCellId="0" sqref="B58"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.337037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.4037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.8296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="32.6333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.0481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.1222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.662962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.5148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="33.4148148148148"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.6333333333333"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4118,9 +4115,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.562962962963"/>
-  </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">

</xml_diff>